<commit_message>
Two tabs (KH1 & KH2) | MP3 compatibility
</commit_message>
<xml_diff>
--- a/resources/All Games Track List - KH2.xlsx
+++ b/resources/All Games Track List - KH2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Kingdom Hearts Modding\KHPCPatchManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Kingdom Hearts Modding\KingdomHeartsCustomMusic\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D5837E-9CFF-4324-8056-2F2E84B15D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3593C5-A0EE-4DBD-AAF4-531DF45EDC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>One Winged Angel</t>
-  </si>
-  <si>
-    <t>Location</t>
   </si>
   <si>
     <t>kh2_fifth</t>
@@ -572,6 +569,9 @@
   <si>
     <t>Battleship Bravery</t>
   </si>
+  <si>
+    <t>Location (.bgm)</t>
+  </si>
 </sst>
 </file>
 
@@ -729,7 +729,24 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
@@ -763,24 +780,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
@@ -870,16 +870,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D8F2C8A-E02E-497E-A16A-A5F88CD5E4E9}" name="Tabla1" displayName="Tabla1" ref="A1:G111" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D8F2C8A-E02E-497E-A16A-A5F88CD5E4E9}" name="Tabla1" displayName="Tabla1" ref="A1:G111" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G111" xr:uid="{8D8F2C8A-E02E-497E-A16A-A5F88CD5E4E9}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2CCDAE5C-2041-488F-BDE2-88973207D649}" name="Location" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{EA90384C-F91D-4D07-9335-173A975FB790}" name="Folder" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{B6EC6AA6-0422-47BB-A055-B254208B7546}" name="PC Number" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{57A90175-4CB2-41F5-A050-D70A493965C7}" name="PlayStation2 Name" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{542F4362-AD27-45AF-B818-FD0A842E8EA0}" name="Description" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{41503F47-36D9-4ACA-AB04-861562B49673}" name="Loop" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{E03880E9-F30F-4FE9-85F4-76159411C872}" name="Full Loop" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{2CCDAE5C-2041-488F-BDE2-88973207D649}" name="Location (.bgm)" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{EA90384C-F91D-4D07-9335-173A975FB790}" name="Folder" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B6EC6AA6-0422-47BB-A055-B254208B7546}" name="PC Number" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{57A90175-4CB2-41F5-A050-D70A493965C7}" name="PlayStation2 Name" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{542F4362-AD27-45AF-B818-FD0A842E8EA0}" name="Description" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{41503F47-36D9-4ACA-AB04-861562B49673}" name="Loop" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{E03880E9-F30F-4FE9-85F4-76159411C872}" name="Full Loop" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1086,12 +1086,12 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="4" max="4" width="31.125" customWidth="1"/>
@@ -1103,7 +1103,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>181</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1146,19 +1146,19 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C2" s="4">
         <v>50</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>7</v>
@@ -1189,10 +1189,10 @@
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C3" s="4">
         <v>51</v>
@@ -1201,7 +1201,7 @@
         <v>31</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>7</v>
@@ -1232,19 +1232,19 @@
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C4" s="4">
         <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>7</v>
@@ -1275,19 +1275,19 @@
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C5" s="4">
         <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>7</v>
@@ -1318,19 +1318,19 @@
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C6" s="4">
         <v>54</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>7</v>
@@ -1361,19 +1361,19 @@
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C7" s="4">
         <v>55</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>7</v>
@@ -1403,16 +1403,16 @@
     </row>
     <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C8" s="4">
         <v>59</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
@@ -1446,16 +1446,16 @@
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C9" s="4">
         <v>60</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>6</v>
@@ -1489,16 +1489,16 @@
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C10" s="4">
         <v>61</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>6</v>
@@ -1532,16 +1532,16 @@
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C11" s="4">
         <v>62</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>6</v>
@@ -1575,16 +1575,16 @@
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C12" s="4">
         <v>63</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>6</v>
@@ -1618,19 +1618,19 @@
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C13" s="4">
         <v>64</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>7</v>
@@ -1661,19 +1661,19 @@
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C14" s="4">
         <v>65</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>7</v>
@@ -1704,16 +1704,16 @@
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C15" s="4">
         <v>66</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>6</v>
@@ -1747,16 +1747,16 @@
     </row>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C16" s="4">
         <v>67</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>6</v>
@@ -1790,19 +1790,19 @@
     </row>
     <row r="17" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C17" s="4">
         <v>68</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>7</v>
@@ -1833,19 +1833,19 @@
     </row>
     <row r="18" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C18" s="4">
         <v>69</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>7</v>
@@ -1876,19 +1876,19 @@
     </row>
     <row r="19" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C19" s="4">
         <v>81</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>7</v>
@@ -1919,19 +1919,19 @@
     </row>
     <row r="20" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="4">
         <v>82</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>7</v>
@@ -1962,19 +1962,19 @@
     </row>
     <row r="21" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C21" s="4">
         <v>84</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>7</v>
@@ -2005,19 +2005,19 @@
     </row>
     <row r="22" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C22" s="4">
         <v>85</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>7</v>
@@ -2048,10 +2048,10 @@
     </row>
     <row r="23" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C23" s="4">
         <v>86</v>
@@ -2060,7 +2060,7 @@
         <v>27</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>7</v>
@@ -2091,10 +2091,10 @@
     </row>
     <row r="24" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C24" s="4">
         <v>87</v>
@@ -2134,16 +2134,16 @@
     </row>
     <row r="25" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C25" s="4">
         <v>88</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>12</v>
@@ -2177,10 +2177,10 @@
     </row>
     <row r="26" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C26" s="4">
         <v>89</v>
@@ -2220,16 +2220,16 @@
     </row>
     <row r="27" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C27" s="4">
         <v>90</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>12</v>
@@ -2263,16 +2263,16 @@
     </row>
     <row r="28" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C28" s="4">
         <v>91</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>12</v>
@@ -2306,10 +2306,10 @@
     </row>
     <row r="29" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C29" s="4">
         <v>92</v>
@@ -2349,16 +2349,16 @@
     </row>
     <row r="30" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C30" s="4">
         <v>93</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>12</v>
@@ -2392,16 +2392,16 @@
     </row>
     <row r="31" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C31" s="4">
         <v>94</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>12</v>
@@ -2435,16 +2435,16 @@
     </row>
     <row r="32" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C32" s="4">
         <v>95</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>12</v>
@@ -2478,16 +2478,16 @@
     </row>
     <row r="33" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C33" s="4">
         <v>96</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>12</v>
@@ -2521,16 +2521,16 @@
     </row>
     <row r="34" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C34" s="4">
         <v>97</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>12</v>
@@ -2564,16 +2564,16 @@
     </row>
     <row r="35" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C35" s="4">
         <v>98</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>12</v>
@@ -2607,16 +2607,16 @@
     </row>
     <row r="36" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C36" s="4">
         <v>99</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>12</v>
@@ -2650,19 +2650,19 @@
     </row>
     <row r="37" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C37" s="4">
         <v>100</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>7</v>
@@ -2693,19 +2693,19 @@
     </row>
     <row r="38" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C38" s="4">
         <v>101</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>7</v>
@@ -2736,19 +2736,19 @@
     </row>
     <row r="39" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C39" s="4">
         <v>102</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>7</v>
@@ -2779,10 +2779,10 @@
     </row>
     <row r="40" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C40" s="4">
         <v>103</v>
@@ -2822,19 +2822,19 @@
     </row>
     <row r="41" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C41" s="4">
         <v>104</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>7</v>
@@ -2865,19 +2865,19 @@
     </row>
     <row r="42" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C42" s="4">
         <v>106</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>8</v>
@@ -2908,19 +2908,19 @@
     </row>
     <row r="43" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C43" s="4">
         <v>107</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>8</v>
@@ -2951,19 +2951,19 @@
     </row>
     <row r="44" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C44" s="4">
         <v>108</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>8</v>
@@ -2994,19 +2994,19 @@
     </row>
     <row r="45" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C45" s="4">
         <v>109</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>8</v>
@@ -3037,19 +3037,19 @@
     </row>
     <row r="46" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C46" s="4">
         <v>110</v>
       </c>
       <c r="D46" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>7</v>
@@ -3080,19 +3080,19 @@
     </row>
     <row r="47" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C47" s="4">
         <v>111</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>7</v>
@@ -3123,19 +3123,19 @@
     </row>
     <row r="48" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C48" s="4">
         <v>112</v>
       </c>
       <c r="D48" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>7</v>
@@ -3166,19 +3166,19 @@
     </row>
     <row r="49" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C49" s="4">
         <v>113</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>8</v>
@@ -3209,19 +3209,19 @@
     </row>
     <row r="50" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C50" s="4">
         <v>114</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>7</v>
@@ -3252,19 +3252,19 @@
     </row>
     <row r="51" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C51" s="4">
         <v>115</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>7</v>
@@ -3295,19 +3295,19 @@
     </row>
     <row r="52" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C52" s="4">
         <v>116</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>7</v>
@@ -3338,19 +3338,19 @@
     </row>
     <row r="53" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C53" s="4">
         <v>117</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>7</v>
@@ -3381,19 +3381,19 @@
     </row>
     <row r="54" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C54" s="4">
         <v>118</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>7</v>
@@ -3424,19 +3424,19 @@
     </row>
     <row r="55" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C55" s="4">
         <v>119</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>7</v>
@@ -3467,19 +3467,19 @@
     </row>
     <row r="56" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C56" s="4">
         <v>120</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>7</v>
@@ -3510,19 +3510,19 @@
     </row>
     <row r="57" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C57" s="4">
         <v>121</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>7</v>
@@ -3553,19 +3553,19 @@
     </row>
     <row r="58" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C58" s="4">
         <v>122</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>7</v>
@@ -3596,19 +3596,19 @@
     </row>
     <row r="59" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C59" s="4">
         <v>123</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>7</v>
@@ -3639,19 +3639,19 @@
     </row>
     <row r="60" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C60" s="4">
         <v>124</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>8</v>
@@ -3682,19 +3682,19 @@
     </row>
     <row r="61" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C61" s="4">
         <v>125</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>8</v>
@@ -3725,16 +3725,16 @@
     </row>
     <row r="62" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C62" s="4">
         <v>127</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>18</v>
@@ -3768,16 +3768,16 @@
     </row>
     <row r="63" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C63" s="4">
         <v>128</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>19</v>
@@ -3811,16 +3811,16 @@
     </row>
     <row r="64" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C64" s="4">
         <v>129</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>21</v>
@@ -3854,19 +3854,19 @@
     </row>
     <row r="65" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C65" s="4">
         <v>130</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>8</v>
@@ -3897,19 +3897,19 @@
     </row>
     <row r="66" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C66" s="4">
         <v>131</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>7</v>
@@ -3940,16 +3940,16 @@
     </row>
     <row r="67" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C67" s="4">
         <v>132</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>12</v>
@@ -3983,19 +3983,19 @@
     </row>
     <row r="68" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C68" s="4">
         <v>133</v>
       </c>
       <c r="D68" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>7</v>
@@ -4026,19 +4026,19 @@
     </row>
     <row r="69" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C69" s="4">
         <v>134</v>
       </c>
       <c r="D69" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>7</v>
@@ -4069,19 +4069,19 @@
     </row>
     <row r="70" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C70" s="4">
         <v>135</v>
       </c>
       <c r="D70" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E70" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>7</v>
@@ -4112,19 +4112,19 @@
     </row>
     <row r="71" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C71" s="4">
         <v>136</v>
       </c>
       <c r="D71" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>7</v>
@@ -4155,16 +4155,16 @@
     </row>
     <row r="72" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C72" s="4">
         <v>137</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>17</v>
@@ -4198,16 +4198,16 @@
     </row>
     <row r="73" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C73" s="4">
         <v>138</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>16</v>
@@ -4241,16 +4241,16 @@
     </row>
     <row r="74" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C74" s="4">
         <v>139</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>16</v>
@@ -4284,10 +4284,10 @@
     </row>
     <row r="75" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C75" s="4">
         <v>141</v>
@@ -4327,16 +4327,16 @@
     </row>
     <row r="76" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C76" s="4">
         <v>142</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>15</v>
@@ -4370,10 +4370,10 @@
     </row>
     <row r="77" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C77" s="4">
         <v>143</v>
@@ -4382,7 +4382,7 @@
         <v>24</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>7</v>
@@ -4413,10 +4413,10 @@
     </row>
     <row r="78" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C78" s="4">
         <v>144</v>
@@ -4456,19 +4456,19 @@
     </row>
     <row r="79" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C79" s="4">
         <v>145</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>7</v>
@@ -4499,16 +4499,16 @@
     </row>
     <row r="80" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C80" s="4">
         <v>146</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>12</v>
@@ -4542,16 +4542,16 @@
     </row>
     <row r="81" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C81" s="4">
         <v>148</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>16</v>
@@ -4585,10 +4585,10 @@
     </row>
     <row r="82" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C82" s="4">
         <v>149</v>
@@ -4597,7 +4597,7 @@
         <v>27</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>7</v>
@@ -4628,19 +4628,19 @@
     </row>
     <row r="83" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C83" s="4">
         <v>151</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>7</v>
@@ -4671,16 +4671,16 @@
     </row>
     <row r="84" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C84" s="4">
         <v>152</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>28</v>
@@ -4714,10 +4714,10 @@
     </row>
     <row r="85" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C85" s="4">
         <v>153</v>
@@ -4757,19 +4757,19 @@
     </row>
     <row r="86" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C86" s="4">
         <v>154</v>
       </c>
       <c r="D86" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E86" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>7</v>
@@ -4800,19 +4800,19 @@
     </row>
     <row r="87" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C87" s="4">
         <v>155</v>
       </c>
       <c r="D87" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>150</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>7</v>
@@ -4843,10 +4843,10 @@
     </row>
     <row r="88" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C88" s="4">
         <v>158</v>
@@ -4886,16 +4886,16 @@
     </row>
     <row r="89" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C89" s="4">
         <v>159</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>33</v>
@@ -4929,10 +4929,10 @@
     </row>
     <row r="90" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C90" s="4">
         <v>164</v>
@@ -4972,16 +4972,16 @@
     </row>
     <row r="91" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C91" s="4">
         <v>185</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>6</v>
@@ -5015,19 +5015,19 @@
     </row>
     <row r="92" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C92" s="4">
         <v>186</v>
       </c>
       <c r="D92" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E92" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>7</v>
@@ -5058,19 +5058,19 @@
     </row>
     <row r="93" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C93" s="4">
         <v>187</v>
       </c>
       <c r="D93" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>156</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>7</v>
@@ -5101,10 +5101,10 @@
     </row>
     <row r="94" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C94" s="4">
         <v>188</v>
@@ -5144,19 +5144,19 @@
     </row>
     <row r="95" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C95" s="4">
         <v>189</v>
       </c>
       <c r="D95" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E95" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>7</v>
@@ -5187,19 +5187,19 @@
     </row>
     <row r="96" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C96" s="4">
         <v>190</v>
       </c>
       <c r="D96" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E96" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>7</v>
@@ -5230,10 +5230,10 @@
     </row>
     <row r="97" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C97" s="4">
         <v>506</v>
@@ -5242,7 +5242,7 @@
         <v>20</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>8</v>
@@ -5273,19 +5273,19 @@
     </row>
     <row r="98" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C98" s="4">
         <v>507</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>8</v>
@@ -5316,19 +5316,19 @@
     </row>
     <row r="99" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C99" s="4">
         <v>508</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>8</v>
@@ -5359,19 +5359,19 @@
     </row>
     <row r="100" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C100" s="4">
         <v>509</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>8</v>
@@ -5402,19 +5402,19 @@
     </row>
     <row r="101" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C101" s="4">
         <v>513</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>8</v>
@@ -5445,19 +5445,19 @@
     </row>
     <row r="102" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C102" s="4">
         <v>517</v>
       </c>
       <c r="D102" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E102" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>7</v>
@@ -5488,19 +5488,19 @@
     </row>
     <row r="103" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C103" s="4">
         <v>521</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>7</v>
@@ -5531,19 +5531,19 @@
     </row>
     <row r="104" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C104" s="4">
         <v>530</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>7</v>
@@ -5574,13 +5574,13 @@
     </row>
     <row r="105" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="C105" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>38</v>
@@ -5617,16 +5617,16 @@
     </row>
     <row r="106" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B106" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="C106" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D106" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>15</v>
@@ -5660,16 +5660,16 @@
     </row>
     <row r="107" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B107" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="C107" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D107" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>15</v>
@@ -5703,16 +5703,16 @@
     </row>
     <row r="108" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B108" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="C108" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D108" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>15</v>
@@ -5746,16 +5746,16 @@
     </row>
     <row r="109" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B109" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="C109" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D109" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>15</v>
@@ -5789,16 +5789,16 @@
     </row>
     <row r="110" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="C110" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D110" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>15</v>
@@ -5832,10 +5832,10 @@
     </row>
     <row r="111" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>14</v>

</xml_diff>